<commit_message>
fixed col widths in export
</commit_message>
<xml_diff>
--- a/Output/AllModels_experimental.xlsx
+++ b/Output/AllModels_experimental.xlsx
@@ -12,21 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="350">
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">Subjective MVPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Device-Based MVPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reactance Gaussian</t>
+    <t xml:space="preserve">Subjective MVPA Hurdle Lognormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device-Based MVPA Lognormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mood Skewnormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reactance Lognormal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reactance Ordinal</t>
   </si>
   <si>
     <t xml:space="preserve">Reactance Dichotome</t>
@@ -122,6 +125,12 @@
     <t xml:space="preserve">[0.89,   1.13]</t>
   </si>
   <si>
+    <t xml:space="preserve">0.68*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.52,  0.87]</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.61*</t>
   </si>
   <si>
@@ -146,6 +155,12 @@
     <t xml:space="preserve">[0.89,   1.12]</t>
   </si>
   <si>
+    <t xml:space="preserve">1.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.76,  1.38]</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.16</t>
   </si>
   <si>
@@ -179,6 +194,12 @@
     <t xml:space="preserve">[0.85,   1.17]</t>
   </si>
   <si>
+    <t xml:space="preserve">1.59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.85,  2.65]</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.03</t>
   </si>
   <si>
@@ -212,6 +233,9 @@
     <t xml:space="preserve">1.18</t>
   </si>
   <si>
+    <t xml:space="preserve">[0.54,  2.41]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[0.26,   5.22]</t>
   </si>
   <si>
@@ -236,6 +260,12 @@
     <t xml:space="preserve">[0.91,   1.15]</t>
   </si>
   <si>
+    <t xml:space="preserve">1.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.98,  1.74]</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.50*</t>
   </si>
   <si>
@@ -263,6 +293,12 @@
     <t xml:space="preserve">[0.81,   1.27]</t>
   </si>
   <si>
+    <t xml:space="preserve">0.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.60,  1.19]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[0.53,   1.61]</t>
   </si>
   <si>
@@ -281,6 +317,12 @@
     <t xml:space="preserve">[0.66,   1.55]</t>
   </si>
   <si>
+    <t xml:space="preserve">1.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.51,  3.90]</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.28</t>
   </si>
   <si>
@@ -323,6 +365,12 @@
     <t xml:space="preserve">[0.43,   1.23]</t>
   </si>
   <si>
+    <t xml:space="preserve">1.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.31,  5.27]</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.29</t>
   </si>
   <si>
@@ -332,9 +380,6 @@
     <t xml:space="preserve">Mean persuasion utilized (partner's view)</t>
   </si>
   <si>
-    <t xml:space="preserve">1.04</t>
-  </si>
-  <si>
     <t xml:space="preserve">[ 0.71,  1.53]</t>
   </si>
   <si>
@@ -353,6 +398,12 @@
     <t xml:space="preserve">[0.70,   1.86]</t>
   </si>
   <si>
+    <t xml:space="preserve">1.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.24,  6.59]</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.62</t>
   </si>
   <si>
@@ -386,6 +437,12 @@
     <t xml:space="preserve">[0.91,   2.46]</t>
   </si>
   <si>
+    <t xml:space="preserve">2.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.40, 10.72]</t>
+  </si>
+  <si>
     <t xml:space="preserve">14.34</t>
   </si>
   <si>
@@ -413,6 +470,9 @@
     <t xml:space="preserve">[0.64,   1.73]</t>
   </si>
   <si>
+    <t xml:space="preserve">[0.17,  5.23]</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.39</t>
   </si>
   <si>
@@ -446,6 +506,12 @@
     <t xml:space="preserve">[0.65,   1.22]</t>
   </si>
   <si>
+    <t xml:space="preserve">1.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.46,  4.08]</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.94</t>
   </si>
   <si>
@@ -470,6 +536,12 @@
     <t xml:space="preserve">[0.71,   1.40]</t>
   </si>
   <si>
+    <t xml:space="preserve">0.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.23,  2.81]</t>
+  </si>
+  <si>
     <t xml:space="preserve">[0.24,   7.26]</t>
   </si>
   <si>
@@ -695,6 +767,9 @@
     <t xml:space="preserve">[0.00, 0.35]</t>
   </si>
   <si>
+    <t xml:space="preserve">[0.59, 1.65]</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.27</t>
   </si>
   <si>
@@ -740,6 +815,12 @@
     <t xml:space="preserve">[0.02, 0.30]</t>
   </si>
   <si>
+    <t xml:space="preserve">0.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.59]</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.47</t>
   </si>
   <si>
@@ -761,6 +842,12 @@
     <t xml:space="preserve">[0.00, 0.18]</t>
   </si>
   <si>
+    <t xml:space="preserve">0.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.69]</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.69</t>
   </si>
   <si>
@@ -782,6 +869,9 @@
     <t xml:space="preserve">[0.00, 0.32]</t>
   </si>
   <si>
+    <t xml:space="preserve">[0.04, 1.41]</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.41</t>
   </si>
   <si>
@@ -803,7 +893,10 @@
     <t xml:space="preserve">[0.01, 1.06]</t>
   </si>
   <si>
-    <t xml:space="preserve">1.21</t>
+    <t xml:space="preserve">0.59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.03, 1.58]</t>
   </si>
   <si>
     <t xml:space="preserve">[0.05, 3.46]</t>
@@ -821,6 +914,12 @@
     <t xml:space="preserve">[0.00, 0.09]</t>
   </si>
   <si>
+    <t xml:space="preserve">0.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 0.74]</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.41</t>
   </si>
   <si>
@@ -836,10 +935,13 @@
     <t xml:space="preserve">[0.00, 0.10]</t>
   </si>
   <si>
-    <t xml:space="preserve">0.22</t>
-  </si>
-  <si>
     <t xml:space="preserve">[0.02, 0.48]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.62]</t>
   </si>
   <si>
     <t xml:space="preserve">0.42</t>
@@ -1355,6 +1457,8 @@
     <col min="9" max="9" width="14.01" hidden="0" customWidth="1"/>
     <col min="10" max="10" width="7.91" hidden="0" customWidth="1"/>
     <col min="11" max="11" width="14.01" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="7.91" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="14.01" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1391,391 +1495,455 @@
       <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="L1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>74</v>
+        <v>81</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="9" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>83</v>
+        <v>94</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="5" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1783,263 +1951,307 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="9" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>114</v>
+        <v>129</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>125</v>
+        <v>142</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>133</v>
+        <v>29</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>134</v>
+        <v>152</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>145</v>
+        <v>165</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>152</v>
+        <v>175</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2047,206 +2259,228 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="9" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="5" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2258,183 +2492,203 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>188</v>
+        <v>212</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
     </row>
     <row r="35">
       <c r="A35" s="9" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
     </row>
     <row r="36">
       <c r="A36" s="9" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
     </row>
     <row r="37">
       <c r="A37" s="9" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
     </row>
     <row r="38">
       <c r="A38" s="9" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2446,486 +2700,556 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="9" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>227</v>
+        <v>110</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>228</v>
+        <v>251</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="9" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
     </row>
     <row r="42">
       <c r="A42" s="9" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>236</v>
+        <v>261</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>238</v>
+        <v>263</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>243</v>
+        <v>268</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="9" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>238</v>
+        <v>263</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>250</v>
+        <v>277</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="9" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>252</v>
+        <v>281</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>254</v>
+        <v>283</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>255</v>
+        <v>284</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>257</v>
+        <v>285</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="9" t="s">
-        <v>258</v>
+        <v>288</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>259</v>
+        <v>289</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>254</v>
+        <v>283</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>261</v>
+        <v>291</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>262</v>
+        <v>292</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>263</v>
+        <v>293</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>264</v>
+        <v>294</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="9" t="s">
-        <v>265</v>
+        <v>296</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>267</v>
+        <v>298</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>269</v>
+        <v>300</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>270</v>
+        <v>301</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="9" t="s">
-        <v>271</v>
+        <v>304</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>272</v>
+        <v>305</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>275</v>
+        <v>307</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>276</v>
+        <v>308</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>277</v>
+        <v>309</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="9" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>279</v>
+        <v>313</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>280</v>
+        <v>314</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1" t="s">
-        <v>281</v>
+        <v>315</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>282</v>
+        <v>316</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
     </row>
     <row r="49">
       <c r="A49" s="9" t="s">
-        <v>283</v>
+        <v>317</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>284</v>
+        <v>318</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>285</v>
+        <v>319</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>286</v>
+        <v>320</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
     </row>
     <row r="50">
       <c r="A50" s="9" t="s">
-        <v>287</v>
+        <v>321</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1" t="s">
-        <v>289</v>
+        <v>323</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>290</v>
+        <v>324</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
     </row>
     <row r="51">
       <c r="A51" s="9" t="s">
-        <v>291</v>
+        <v>325</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>292</v>
+        <v>326</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>293</v>
+        <v>327</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1" t="s">
-        <v>294</v>
+        <v>328</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>295</v>
+        <v>329</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
     </row>
     <row r="52">
       <c r="A52" s="9" t="s">
-        <v>296</v>
+        <v>330</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>297</v>
+        <v>331</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>298</v>
+        <v>332</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1" t="s">
-        <v>269</v>
+        <v>302</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>299</v>
+        <v>333</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
     </row>
     <row r="53">
       <c r="A53" s="9" t="s">
-        <v>300</v>
+        <v>334</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>301</v>
+        <v>335</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>302</v>
+        <v>336</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1" t="s">
-        <v>269</v>
+        <v>302</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>303</v>
+        <v>337</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
     </row>
     <row r="54">
       <c r="A54" s="8" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>304</v>
+        <v>338</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="9" t="s">
-        <v>305</v>
+        <v>339</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2937,10 +3261,12 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
     </row>
     <row r="56">
       <c r="A56" s="9" t="s">
-        <v>306</v>
+        <v>340</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2952,10 +3278,12 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
     </row>
     <row r="57">
       <c r="A57" s="9" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2967,10 +3295,12 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
     </row>
     <row r="58">
       <c r="A58" s="9" t="s">
-        <v>308</v>
+        <v>342</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2982,37 +3312,41 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
     </row>
     <row r="59">
       <c r="A59" s="10" t="s">
-        <v>309</v>
+        <v>343</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>310</v>
+        <v>344</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>312</v>
+        <v>346</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>313</v>
+        <v>347</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>314</v>
+        <v>348</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>315</v>
+        <v>349</v>
       </c>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
     </row>
     <row r="60">
       <c r="A60" s="9"/>
@@ -3042,120 +3376,152 @@
       <c r="A68" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="113">
+  <mergeCells count="145">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="J3:K3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:M27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:M28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="J35:K35"/>
+    <mergeCell ref="L35:M35"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="J36:K36"/>
+    <mergeCell ref="L36:M36"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="F48:G48"/>
     <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L48:M48"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="J49:K49"/>
+    <mergeCell ref="L49:M49"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="F50:G50"/>
     <mergeCell ref="J50:K50"/>
+    <mergeCell ref="L50:M50"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="J51:K51"/>
+    <mergeCell ref="L51:M51"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="J52:K52"/>
+    <mergeCell ref="L52:M52"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="F53:G53"/>
     <mergeCell ref="J53:K53"/>
+    <mergeCell ref="L53:M53"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="F55:G55"/>
     <mergeCell ref="H55:I55"/>
     <mergeCell ref="J55:K55"/>
+    <mergeCell ref="L55:M55"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="F56:G56"/>
     <mergeCell ref="H56:I56"/>
     <mergeCell ref="J56:K56"/>
+    <mergeCell ref="L56:M56"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="D57:E57"/>
     <mergeCell ref="F57:G57"/>
     <mergeCell ref="H57:I57"/>
     <mergeCell ref="J57:K57"/>
+    <mergeCell ref="L57:M57"/>
     <mergeCell ref="B58:C58"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="F58:G58"/>
     <mergeCell ref="H58:I58"/>
     <mergeCell ref="J58:K58"/>
+    <mergeCell ref="L58:M58"/>
     <mergeCell ref="J59:K59"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A22:M22"/>
+    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="A54:M54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
ran all experimental models mean machine
</commit_message>
<xml_diff>
--- a/Output/AllModels_experimental.xlsx
+++ b/Output/AllModels_experimental.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="347">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -50,10 +50,10 @@
     <t xml:space="preserve">Intercept</t>
   </si>
   <si>
-    <t xml:space="preserve">55.19*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[45.47, 65.79]</t>
+    <t xml:space="preserve">54.95*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[45.92, 65.49]</t>
   </si>
   <si>
     <t xml:space="preserve">121.53*</t>
@@ -65,19 +65,19 @@
     <t xml:space="preserve">4.90*</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 4.78, 5.01]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.93*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.47,   2.52]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.28,   1.52]</t>
+    <t xml:space="preserve">[ 4.79, 5.01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.94*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.48,   2.51]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.27,   1.44]</t>
   </si>
   <si>
     <t xml:space="preserve">Hurdle Intercept</t>
@@ -86,13 +86,13 @@
     <t xml:space="preserve">0.32*</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.18,  0.57]</t>
+    <t xml:space="preserve">[ 0.18,  0.58]</t>
   </si>
   <si>
     <t xml:space="preserve">4.72*</t>
   </si>
   <si>
-    <t xml:space="preserve">[1.76,  13.70]</t>
+    <t xml:space="preserve">[1.72,  13.64]</t>
   </si>
   <si>
     <t xml:space="preserve">Conditional Within-Person Effects</t>
@@ -122,49 +122,46 @@
     <t xml:space="preserve">0.99</t>
   </si>
   <si>
+    <t xml:space="preserve">[0.89,   1.12]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.67*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.52,  0.86]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.62*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.42,   0.86]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.97,  1.08]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.03, 0.02]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.01</t>
+  </si>
+  <si>
     <t xml:space="preserve">[0.89,   1.13]</t>
   </si>
   <si>
-    <t xml:space="preserve">0.68*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.52,  0.87]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.61*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.40,   0.85]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.97,  1.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.03, 0.02]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.89,   1.12]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.76,  1.38]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.73,   1.98]</t>
+    <t xml:space="preserve">[0.74,  1.38]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.75,   1.99]</t>
   </si>
   <si>
     <t xml:space="preserve">Daily pressure experienced</t>
@@ -173,7 +170,7 @@
     <t xml:space="preserve">0.89</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.78,  1.01]</t>
+    <t xml:space="preserve">[ 0.77,  1.01]</t>
   </si>
   <si>
     <t xml:space="preserve">0.96</t>
@@ -185,25 +182,25 @@
     <t xml:space="preserve">-0.02</t>
   </si>
   <si>
-    <t xml:space="preserve">[-0.11, 0.08]</t>
+    <t xml:space="preserve">[-0.12, 0.09]</t>
   </si>
   <si>
     <t xml:space="preserve">1.00</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.85,   1.17]</t>
+    <t xml:space="preserve">[0.84,   1.18]</t>
   </si>
   <si>
     <t xml:space="preserve">1.59</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.85,  2.65]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.73,   8.23]</t>
+    <t xml:space="preserve">[0.86,  2.72]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.69,   7.63]</t>
   </si>
   <si>
     <t xml:space="preserve">Daily pressure utilized (partner's view)</t>
@@ -212,7 +209,7 @@
     <t xml:space="preserve">0.92</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.81,  1.03]</t>
+    <t xml:space="preserve">[ 0.82,  1.04]</t>
   </si>
   <si>
     <t xml:space="preserve">0.93</t>
@@ -227,832 +224,826 @@
     <t xml:space="preserve">[-0.20, 0.05]</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.63,   1.51]</t>
+    <t xml:space="preserve">[0.61,   1.60]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.50,  2.37]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.30,   6.13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.92,  1.04]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.96,   1.09]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.02, 0.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.91,   1.16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.95,  1.76]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.49*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.04,   2.30]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.90,  1.03]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.97,   1.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.01, 0.08]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.82,   1.24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.58,  1.20]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.53,   1.64]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.79,  1.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.89,   1.11]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.11, 0.06]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.65,   1.54]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.49,  3.87]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.41,   4.00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.00*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  1.00,   1.00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional Between-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.74,  1.62]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.79,   1.50]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.19, 0.35]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.42,   1.22]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.30,  4.97]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.51,  23.74]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.71,  1.56]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.65,   1.24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.25, 0.32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.67,   1.85]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.26,  5.72]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.37,  20.54]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean pressure experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.38,  1.89]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.55,   1.12]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.38, 0.24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.89,   2.55]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.42, 10.70]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.80, 300.95]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.32,  1.53]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.71,   1.41]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.31, 0.31]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.63,   1.76]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.19,  5.53]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02,   8.81]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.85,  1.69]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[  0.84,   1.43]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.24, 0.24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.66,   1.25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.43,  3.78]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.43,   9.84]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.83,  1.65]</t>
   </si>
   <si>
     <t xml:space="preserve">1.18</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.54,  2.41]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.26,   5.22]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.92,  1.04]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.96,   1.09]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.02, 0.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.91,   1.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.98,  1.74]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.50*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.04,   2.34]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.91,  1.03]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.97,   1.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.01, 0.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.81,   1.27]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.60,  1.19]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.53,   1.61]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.79,  1.07]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.89,   1.11]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.10, 0.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.66,   1.55]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.51,  3.90]</t>
+    <t xml:space="preserve">[  0.90,   1.52]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.19, 0.29]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.72,   1.42]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.22,  2.62]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.24,   7.02]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hurdle Within-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.65*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.50,  0.81]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.54*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.11,   2.27]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.75*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.59,  0.93]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.65,   1.73]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pressure experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.77,  2.96]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.19,   1.67]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.11,  1.96]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.19,   6.01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.45,  0.95]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.49,   1.03]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.58*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.35,  0.84]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.71,   1.96]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Day</t>
   </si>
   <si>
     <t xml:space="preserve">1.28</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.40,   4.04]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.00*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  1.00,   1.00]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conditional Between-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.73,  1.59]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.79,   1.50]</t>
+    <t xml:space="preserve">[ 0.75,  2.18]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.22,   2.54]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Daily weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hurdle Between-Person Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean persuasion experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.13,  3.01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.07,   4.65]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean persuasion utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.14,  3.21]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.06,   6.28]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pressure experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.62, 37.00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00,   1.39]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pressure utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.51, 31.63]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.14, 174.07]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pushing experienced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.45,  5.61]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.15,   3.75]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean pushing utilized (partner's view)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.32,  4.05]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.21,   7.27]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hu Mean weartime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random Effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.28, 0.50]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.25, 0.42]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.21, 0.37]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.36]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.57, 1.66]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.46, 3.32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hurdle Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.06, 2.02]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.95, 3.02]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily persuasion experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.04, 0.15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.11]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.06]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 0.31]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.58]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.07, 0.92]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily persuasion utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 0.14]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.04]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.19]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.69]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.10, 1.45]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily pressure experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.28]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.06, 1.44]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.17, 3.21]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily pressure utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.29]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 1.22]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.03, 1.61]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.06, 3.43]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily pushing experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.17]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.09]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 0.78]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 0.97]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Daily pushing utilized (partner's view))</t>
   </si>
   <si>
     <t xml:space="preserve">0.07</t>
   </si>
   <si>
-    <t xml:space="preserve">[-0.18, 0.36]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.43,   1.23]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.31,  5.27]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.42,  24.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.71,  1.53]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.65,   1.24]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.24, 0.33]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.70,   1.86]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.24,  6.59]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.37,  21.27]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean pressure experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.36,  2.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.55,   1.12]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.38, 0.24]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.91,   2.46]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.40, 10.72]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.82, 297.90]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.30,  1.67]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.71,   1.41]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.31, 0.32]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.64,   1.73]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.17,  5.23]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02,   8.90]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.87,  1.70]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.84,   1.43]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.23, 0.24]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.65,   1.22]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.46,  4.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.42,   9.37]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.83,  1.65]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[  0.90,   1.52]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.19, 0.30]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.71,   1.40]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.23,  2.81]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.24,   7.26]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hurdle Within-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.65*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.49,  0.81]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.54*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.12,   2.28]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.75*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.61,  0.93]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.62,   1.72]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily pressure experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.77,  2.99]</t>
+    <t xml:space="preserve">[0.01, 0.16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00, 0.10]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 0.45]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.63]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 1.17]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily persuasion experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.61]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.05, 0.92]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily persuasion utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.55]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.08, 1.43]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily pressure experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 1.74]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.20, 3.47]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily pressure utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.08, 3.83]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.06, 4.46]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily pushing experienced)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.05, 1.09]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 1.00]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sd(Hu Daily pushing utilized (partner's view))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.04, 1.24]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.02, 1.15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ar[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sderr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.63, 0.69]</t>
   </si>
   <si>
     <t xml:space="preserve">0.54</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.16,   1.49]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.11,  1.87]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.18,   6.49]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.67*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.45,  0.95]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.49,   1.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.58*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.37,  0.84]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.70,   2.00]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.75,  2.09]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.23,   2.47]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Daily weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hurdle Between-Person Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean persuasion experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.15,  3.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.05,   4.23]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean persuasion utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.15,  3.31]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.06,   6.11]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pressure experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.67, 33.59]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00,   1.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pressure utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.52, 25.65]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.18, 139.61]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pushing experienced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.45,  5.58]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.18,   3.52]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean pushing utilized (partner's view)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.31,  4.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.22,   7.68]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hu Mean weartime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Random Effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Intercept)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.28, 0.50]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.25, 0.42]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.21, 0.37]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.35]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.59, 1.65]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.48, 3.29]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hurdle Intercept)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.06, 2.01]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.92, 2.99]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily persuasion experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.04, 0.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.11]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.30]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.59]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.07, 0.93]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily persuasion utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.14]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.04]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.18]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.69]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.11, 1.43]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily pressure experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.27]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.24]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.32]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.04, 1.41]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.18, 3.21]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily pressure utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.30]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 1.06]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.03, 1.58]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.05, 3.46]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily pushing experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.13]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.09]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.74]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.03, 0.99]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Daily pushing utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.16]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.10]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.48]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.62]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 1.17]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily persuasion experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.60]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.05, 0.94]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily persuasion utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.54]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.10, 1.46]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily pressure experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 1.64]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.11, 3.49]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily pressure utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.09, 3.76]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.07, 4.61]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily pushing experienced)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.06, 1.05]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 0.96]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sd(Hu Daily pushing utilized (partner's view))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.03, 1.21]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.02, 1.08]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ar[1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sderr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sigma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.63, 0.69]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[0.52, 0.56]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.85</t>
   </si>
   <si>
     <t xml:space="preserve">[0.82, 0.89]</t>
@@ -1716,95 +1707,95 @@
         <v>46</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>74</v>
@@ -1874,7 +1865,7 @@
         <v>91</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>92</v>
@@ -1886,48 +1877,48 @@
         <v>94</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>104</v>
@@ -2006,249 +1997,249 @@
         <v>111</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>123</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>137</v>
+        <v>68</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>151</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>29</v>
+        <v>152</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>157</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="L19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="H20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="L20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>107</v>
@@ -2264,64 +2255,64 @@
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -2330,13 +2321,13 @@
     </row>
     <row r="24">
       <c r="A24" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -2346,7 +2337,7 @@
         <v>31</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -2355,23 +2346,23 @@
     </row>
     <row r="25">
       <c r="A25" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -2380,23 +2371,23 @@
     </row>
     <row r="26">
       <c r="A26" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>196</v>
+        <v>66</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -2405,23 +2396,23 @@
     </row>
     <row r="27">
       <c r="A27" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -2430,23 +2421,23 @@
     </row>
     <row r="28">
       <c r="A28" s="9" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2455,23 +2446,23 @@
     </row>
     <row r="29">
       <c r="A29" s="9" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2480,7 +2471,7 @@
     </row>
     <row r="30">
       <c r="A30" s="9" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2497,64 +2488,64 @@
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -2563,23 +2554,23 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -2588,23 +2579,23 @@
     </row>
     <row r="34">
       <c r="A34" s="9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>171</v>
+        <v>220</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -2613,23 +2604,23 @@
     </row>
     <row r="35">
       <c r="A35" s="9" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2638,23 +2629,23 @@
     </row>
     <row r="36">
       <c r="A36" s="9" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>233</v>
+        <v>59</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -2663,23 +2654,23 @@
     </row>
     <row r="37">
       <c r="A37" s="9" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>237</v>
+        <v>71</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2688,7 +2679,7 @@
     </row>
     <row r="38">
       <c r="A38" s="9" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2705,105 +2696,105 @@
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="J40" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K40" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="M40" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="9" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -2812,269 +2803,269 @@
     </row>
     <row r="42">
       <c r="A42" s="9" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="L43" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="M43" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M44" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="M45" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="9" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>171</v>
+        <v>266</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>90</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="K47" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="9" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -3083,23 +3074,23 @@
     </row>
     <row r="49">
       <c r="A49" s="9" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -3108,23 +3099,23 @@
     </row>
     <row r="50">
       <c r="A50" s="9" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>191</v>
+        <v>317</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -3133,23 +3124,23 @@
     </row>
     <row r="51">
       <c r="A51" s="9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -3158,23 +3149,23 @@
     </row>
     <row r="52">
       <c r="A52" s="9" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -3183,23 +3174,23 @@
     </row>
     <row r="53">
       <c r="A53" s="9" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1" t="s">
-        <v>302</v>
+        <v>332</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -3208,48 +3199,48 @@
     </row>
     <row r="54">
       <c r="A54" s="8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="9" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3266,7 +3257,7 @@
     </row>
     <row r="56">
       <c r="A56" s="9" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3283,7 +3274,7 @@
     </row>
     <row r="57">
       <c r="A57" s="9" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3300,7 +3291,7 @@
     </row>
     <row r="58">
       <c r="A58" s="9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3317,31 +3308,31 @@
     </row>
     <row r="59">
       <c r="A59" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="E59" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="C59" s="4" t="s">
+      <c r="F59" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G59" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="D59" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E59" s="4" t="s">
+      <c r="H59" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="I59" s="4" t="s">
         <v>346</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>349</v>
       </c>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>

</xml_diff>